<commit_message>
[Done] IsVe & PPT
</commit_message>
<xml_diff>
--- a/DP2.xlsx
+++ b/DP2.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\User\Desktop\Dynamic_Programming\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL\參考\Dynamic Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46415352-01F8-4CD9-9CFF-6D9AF36855DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DP (2)" sheetId="9" r:id="rId1"/>
@@ -22,7 +21,7 @@
     <sheet name="原數據" sheetId="1" r:id="rId7"/>
     <sheet name="更改後數據" sheetId="2" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="101">
   <si>
     <t>品項</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -386,13 +385,45 @@
   </si>
   <si>
     <t>第幾天</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>葷素</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>神奇沙拉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>葷</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>素</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>我是素食</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>素肉全餐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>涼麵(素)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>餐點</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="176" formatCode="0.00_ "/>
     <numFmt numFmtId="177" formatCode="0.00000000000_ "/>
@@ -1043,11 +1074,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80AFA412-316E-462E-AEF2-CB88A3843F82}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="A1:G13"/>
+      <selection activeCell="E13" sqref="A1:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1319,19 +1350,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L24" sqref="K24:L25"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9" style="15"/>
+    <col min="1" max="1" width="15.75" style="15" customWidth="1"/>
+    <col min="2" max="4" width="9" style="15"/>
+    <col min="5" max="5" width="14" style="15" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>100</v>
+      </c>
       <c r="B1" s="15" t="s">
         <v>38</v>
       </c>
@@ -1344,8 +1381,11 @@
       <c r="E1" s="15" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>40</v>
       </c>
@@ -1361,10 +1401,13 @@
       <c r="E2" s="15">
         <v>90</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>41</v>
+        <v>97</v>
       </c>
       <c r="B3" s="15">
         <v>875</v>
@@ -1378,10 +1421,13 @@
       <c r="E3" s="15">
         <v>79</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="15" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>42</v>
+        <v>94</v>
       </c>
       <c r="B4" s="15">
         <v>716</v>
@@ -1395,8 +1441,11 @@
       <c r="E4" s="15">
         <v>70</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="15" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>43</v>
       </c>
@@ -1412,49 +1461,179 @@
       <c r="E5" s="15">
         <v>68</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="15">
+        <v>570</v>
+      </c>
+      <c r="C6" s="15">
+        <v>110</v>
+      </c>
+      <c r="D6" s="15">
+        <v>71</v>
+      </c>
+      <c r="E6" s="15">
+        <v>67</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="15">
+        <v>550</v>
+      </c>
+      <c r="C7" s="15">
+        <v>120</v>
+      </c>
+      <c r="D7" s="15">
+        <v>69</v>
+      </c>
+      <c r="E7" s="15">
+        <v>65</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="15">
+        <v>450</v>
+      </c>
+      <c r="C8" s="15">
+        <v>135</v>
+      </c>
+      <c r="D8" s="15">
+        <v>68</v>
+      </c>
+      <c r="E8" s="15">
+        <v>66</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" s="15">
+        <v>440</v>
+      </c>
+      <c r="C9" s="15">
+        <v>105</v>
+      </c>
+      <c r="D9" s="15">
+        <v>65</v>
+      </c>
+      <c r="E9" s="15">
+        <v>63</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10" s="15">
+        <v>380</v>
+      </c>
+      <c r="C10" s="15">
+        <v>60</v>
+      </c>
+      <c r="D10" s="15">
+        <v>62</v>
+      </c>
+      <c r="E10" s="15">
+        <v>61</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B11" s="15">
         <v>370</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C11" s="15">
         <v>70</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D11" s="15">
         <v>59</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E11" s="15">
         <v>58</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="F11" s="15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B12" s="15">
         <v>300</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C12" s="15">
         <v>65</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D12" s="15">
         <v>53</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E12" s="15">
         <v>53</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="15">
+        <v>300</v>
+      </c>
+      <c r="C13" s="15">
+        <v>60</v>
+      </c>
+      <c r="D13" s="15">
+        <v>50</v>
+      </c>
+      <c r="E13" s="15">
+        <v>50</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:W36"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
@@ -3335,7 +3514,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3947,7 +4126,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4796,7 +4975,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:V56"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
@@ -6160,7 +6339,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:P28"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -6898,7 +7077,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:P28"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -7623,7 +7802,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:F16">
+  <sortState ref="A5:F16">
     <sortCondition descending="1" ref="B5:B16"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>